<commit_message>
PDP and FPP update
</commit_message>
<xml_diff>
--- a/BP8/Rev3/Derating.xlsx
+++ b/BP8/Rev3/Derating.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="377">
   <si>
     <t>Designator</t>
   </si>
@@ -1125,6 +1125,36 @@
   </si>
   <si>
     <t>CAP CER 15PF 100V 0603</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>AEC Q200</t>
+  </si>
+  <si>
+    <t>COTS</t>
+  </si>
+  <si>
+    <t>AEC-Q101</t>
+  </si>
+  <si>
+    <t>COTS -40 to 125</t>
+  </si>
+  <si>
+    <t>COTS -55 to 125</t>
+  </si>
+  <si>
+    <t>COTS -65 to 150</t>
+  </si>
+  <si>
+    <t>COTS -40 to 85</t>
+  </si>
+  <si>
+    <t>COTS -55 to 150</t>
+  </si>
+  <si>
+    <t>COTS -55 to 175</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1240,11 +1270,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1300,6 +1341,17 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1616,10 +1668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1634,9 +1686,10 @@
     <col min="8" max="8" width="7.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -1667,8 +1720,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K1" s="21" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1695,8 +1751,11 @@
         <v>16</v>
       </c>
       <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K2" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1723,8 +1782,11 @@
         <v>16</v>
       </c>
       <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -1751,8 +1813,11 @@
         <v>16</v>
       </c>
       <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K4" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
@@ -1779,8 +1844,11 @@
         <v>16</v>
       </c>
       <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K5" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1807,8 +1875,11 @@
         <v>16</v>
       </c>
       <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K6" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -1835,8 +1906,11 @@
         <v>16</v>
       </c>
       <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
@@ -1863,8 +1937,11 @@
         <v>16</v>
       </c>
       <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
@@ -1891,8 +1968,11 @@
         <v>16</v>
       </c>
       <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
@@ -1919,8 +1999,11 @@
         <v>16</v>
       </c>
       <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1947,8 +2030,11 @@
         <v>16</v>
       </c>
       <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -1975,8 +2061,11 @@
         <v>16</v>
       </c>
       <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>53</v>
       </c>
@@ -2003,8 +2092,11 @@
         <v>16</v>
       </c>
       <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="K13" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>56</v>
       </c>
@@ -2031,8 +2123,11 @@
         <v>16</v>
       </c>
       <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K14" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>62</v>
       </c>
@@ -2059,8 +2154,11 @@
         <v>16</v>
       </c>
       <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K15" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
@@ -2087,8 +2185,11 @@
         <v>16</v>
       </c>
       <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="23" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>72</v>
       </c>
@@ -2115,8 +2216,11 @@
         <v>16</v>
       </c>
       <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K17" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>77</v>
       </c>
@@ -2143,8 +2247,11 @@
         <v>16</v>
       </c>
       <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K18" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>83</v>
       </c>
@@ -2171,8 +2278,11 @@
         <v>16</v>
       </c>
       <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K19" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>86</v>
       </c>
@@ -2199,8 +2309,11 @@
         <v>16</v>
       </c>
       <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>89</v>
       </c>
@@ -2227,8 +2340,11 @@
         <v>16</v>
       </c>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K21" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>95</v>
       </c>
@@ -2255,8 +2371,11 @@
         <v>100</v>
       </c>
       <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K22" s="25" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>102</v>
       </c>
@@ -2283,8 +2402,11 @@
         <v>105</v>
       </c>
       <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K23" s="25" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>107</v>
       </c>
@@ -2311,8 +2433,11 @@
         <v>105</v>
       </c>
       <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="K24" s="25" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>110</v>
       </c>
@@ -2339,8 +2464,11 @@
         <v>16</v>
       </c>
       <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K25" s="25" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>115</v>
       </c>
@@ -2367,8 +2495,11 @@
         <v>16</v>
       </c>
       <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K26" s="23" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>119</v>
       </c>
@@ -2395,8 +2526,11 @@
         <v>16</v>
       </c>
       <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>123</v>
       </c>
@@ -2423,8 +2557,11 @@
         <v>16</v>
       </c>
       <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K28" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>129</v>
       </c>
@@ -2451,8 +2588,11 @@
         <v>16</v>
       </c>
       <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K29" s="24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>134</v>
       </c>
@@ -2479,8 +2619,11 @@
         <v>16</v>
       </c>
       <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K30" s="25" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>139</v>
       </c>
@@ -2509,8 +2652,11 @@
       <c r="J31" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="K31" s="25" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>145</v>
       </c>

</xml_diff>